<commit_message>
Calculator data set if valid. Only problem is going to be with accidents PAF caluculation.
</commit_message>
<xml_diff>
--- a/files/osa_prevalence_country_specific.xlsx
+++ b/files/osa_prevalence_country_specific.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/japmiett/projects/sleep22/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/japmiett/projects/sleep22/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21F17C44-9C0D-4C43-A836-397879A7E735}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAED0A6B-22F3-034D-BF9B-1E2D2D7A096E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4140" yWindow="500" windowWidth="27480" windowHeight="19640" xr2:uid="{2643E2FA-F612-4AF1-B2D6-5928DCE52AD2}"/>
+    <workbookView xWindow="4140" yWindow="500" windowWidth="27480" windowHeight="19380" xr2:uid="{2643E2FA-F612-4AF1-B2D6-5928DCE52AD2}"/>
   </bookViews>
   <sheets>
     <sheet name="final" sheetId="4" r:id="rId1"/>
-    <sheet name="Sheet1 (3)" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet1 (2)" sheetId="2" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="percentages" sheetId="3" r:id="rId2"/>
+    <sheet name="cleaned" sheetId="2" r:id="rId3"/>
+    <sheet name="original" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -2453,7 +2453,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2475,7 +2475,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2804,23 +2803,23 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.1640625" style="7" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="48" x14ac:dyDescent="0.2">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>787</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="10" t="s">
         <v>786</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="10" t="s">
         <v>789</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="10" t="s">
         <v>790</v>
       </c>
     </row>
@@ -12535,7 +12534,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B436128C-F83D-704D-B54D-64D45ABE51D1}">
   <dimension ref="A1:J194"/>
   <sheetViews>
-    <sheetView topLeftCell="A39" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I68" sqref="I68"/>
     </sheetView>
   </sheetViews>

</xml_diff>